<commit_message>
Updated notes for day 2 and practical 4
</commit_message>
<xml_diff>
--- a/practicals/other_data_sets.xlsx
+++ b/practicals/other_data_sets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GDrive/IDA/DAFM/practicals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/intro_stats_with_excel/practicals/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Driving speeds (mph)</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>x bar bar</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>Rbar</t>
   </si>
 </sst>
 </file>
@@ -1323,13 +1332,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
@@ -1340,7 +1351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1351,7 +1362,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1362,7 +1373,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -1373,7 +1384,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -1384,7 +1395,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -1395,7 +1406,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -1405,8 +1416,15 @@
       <c r="C7" s="15">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <f>AVERAGE(B2:B21)</f>
+        <v>4.2155000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -1416,8 +1434,14 @@
       <c r="C8" s="15">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1427,8 +1451,15 @@
       <c r="C9" s="15">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(C2:C21)</f>
+        <v>0.15550000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -1439,7 +1470,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -1450,7 +1481,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -1461,7 +1492,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -1472,7 +1503,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -1483,7 +1514,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -1494,7 +1525,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <v>15</v>
       </c>

</xml_diff>